<commit_message>
Mover 0 a 1 Quick
</commit_message>
<xml_diff>
--- a/Software Comparador/Calibraciones en curso/2024-02-12_Datos.xlsx
+++ b/Software Comparador/Calibraciones en curso/2024-02-12_Datos.xlsx
@@ -374,7 +374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:O500"/>
+  <dimension ref="A1:S500"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
@@ -504,61 +504,229 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t>002</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="4" t="n">
         <v>20.679</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="4" t="n">
         <v>21.014</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" s="4" t="n">
         <v>21.074</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="4" t="n">
         <v>20.772</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="4" t="n">
         <v>51.92</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="4" t="n">
         <v>20.68</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" s="4" t="n">
         <v>21.024</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" s="4" t="n">
         <v>21.083</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3" s="4" t="n">
         <v>20.773</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" s="4" t="n">
         <v>51.76</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3" s="4" t="n">
         <v>1000</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3" s="4" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>001</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>20.796</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>21.144</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>21.16</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>20.855</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>57.06</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>20.774</v>
+      </c>
+      <c r="J4" s="4" t="n">
+        <v>21.123</v>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>21.156</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>20.849</v>
+      </c>
+      <c r="M4" s="4" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="N4" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O4" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P4" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="Q4" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R4" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S4" s="4" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>002</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>20.826</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>21.241</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>21.225</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>20.897</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>56.68</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>20.833</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>21.25</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>21.231</v>
+      </c>
+      <c r="L5" s="4" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <v>56.66</v>
+      </c>
+      <c r="N5" s="4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>003</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>20.84</v>
+      </c>
+      <c r="E6" t="n">
+        <v>21.27</v>
+      </c>
+      <c r="F6" t="n">
+        <v>21.237</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20.911</v>
+      </c>
+      <c r="H6" t="n">
+        <v>56.53</v>
+      </c>
+      <c r="I6" t="n">
+        <v>20.837</v>
+      </c>
+      <c r="J6" t="n">
+        <v>21.265</v>
+      </c>
+      <c r="K6" t="n">
+        <v>21.235</v>
+      </c>
+      <c r="L6" t="n">
+        <v>20.912</v>
+      </c>
+      <c r="M6" t="n">
+        <v>56.55</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1000</v>
+      </c>
+    </row>
     <row r="7"/>
     <row r="8"/>
     <row r="9"/>

</xml_diff>